<commit_message>
(by Lorenzo) fix the data
</commit_message>
<xml_diff>
--- a/Fenocchio_ULTERA_Contribute.xlsx
+++ b/Fenocchio_ULTERA_Contribute.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loren\ULTERA-contribute\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loren\ULTREA_MongoDB\ULTERA\ULTERA-contribute\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A635262-4396-4F2E-B2A9-686C1310DBF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF16DD8E-B930-4D6B-899A-D9796E553462}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1155,7 +1155,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1232,6 +1232,14 @@
       <sz val="8"/>
       <color theme="0" tint="-0.499984740745262"/>
       <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="9">
@@ -1717,7 +1725,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1834,6 +1842,33 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1885,33 +1920,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="11" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Collegamento ipertestuale" xfId="1" builtinId="8"/>
@@ -2195,8 +2204,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T430"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="90" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F213" sqref="F213"/>
+    <sheetView tabSelected="1" topLeftCell="D175" zoomScale="70" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="J199" sqref="J199"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
@@ -2232,21 +2241,21 @@
       <c r="B2" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="D2" s="46" t="s">
+      <c r="D2" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="47"/>
-      <c r="F2" s="42" t="s">
+      <c r="E2" s="56"/>
+      <c r="F2" s="51" t="s">
         <v>286</v>
       </c>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
-      <c r="I2" s="42"/>
-      <c r="J2" s="42"/>
-      <c r="K2" s="42"/>
-      <c r="L2" s="42"/>
-      <c r="M2" s="42"/>
-      <c r="N2" s="43"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="51"/>
+      <c r="K2" s="51"/>
+      <c r="L2" s="51"/>
+      <c r="M2" s="51"/>
+      <c r="N2" s="52"/>
       <c r="O2" s="26"/>
     </row>
     <row r="3" spans="1:20" ht="22.05" customHeight="1" thickBot="1">
@@ -2256,17 +2265,17 @@
       <c r="B3" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="D3" s="48"/>
-      <c r="E3" s="49"/>
-      <c r="F3" s="44"/>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
-      <c r="J3" s="44"/>
-      <c r="K3" s="44"/>
-      <c r="L3" s="44"/>
-      <c r="M3" s="44"/>
-      <c r="N3" s="45"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="58"/>
+      <c r="F3" s="53"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="53"/>
+      <c r="I3" s="53"/>
+      <c r="J3" s="53"/>
+      <c r="K3" s="53"/>
+      <c r="L3" s="53"/>
+      <c r="M3" s="53"/>
+      <c r="N3" s="54"/>
       <c r="O3" s="26"/>
     </row>
     <row r="4" spans="1:20" ht="22.5" customHeight="1">
@@ -2284,43 +2293,43 @@
       <c r="B5" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="58" t="s">
+      <c r="C5" s="67" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="59" t="s">
+      <c r="D5" s="48" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="59" t="s">
+      <c r="E5" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="59" t="s">
+      <c r="F5" s="48" t="s">
         <v>53</v>
       </c>
-      <c r="G5" s="59" t="s">
+      <c r="G5" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="66" t="s">
+      <c r="H5" s="49" t="s">
         <v>230</v>
       </c>
-      <c r="I5" s="59" t="s">
+      <c r="I5" s="48" t="s">
         <v>55</v>
       </c>
-      <c r="J5" s="59" t="s">
+      <c r="J5" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="K5" s="59" t="s">
+      <c r="K5" s="48" t="s">
         <v>45</v>
       </c>
-      <c r="L5" s="59" t="s">
+      <c r="L5" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="M5" s="59" t="s">
+      <c r="M5" s="48" t="s">
         <v>56</v>
       </c>
-      <c r="N5" s="59" t="s">
+      <c r="N5" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="O5" s="60" t="s">
+      <c r="O5" s="42" t="s">
         <v>49</v>
       </c>
     </row>
@@ -2331,19 +2340,19 @@
       <c r="B6" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="59"/>
-      <c r="D6" s="59"/>
-      <c r="E6" s="59"/>
-      <c r="F6" s="59"/>
-      <c r="G6" s="59"/>
-      <c r="H6" s="67"/>
-      <c r="I6" s="59"/>
-      <c r="J6" s="59"/>
-      <c r="K6" s="59"/>
-      <c r="L6" s="59"/>
-      <c r="M6" s="59"/>
-      <c r="N6" s="59"/>
-      <c r="O6" s="61"/>
+      <c r="C6" s="48"/>
+      <c r="D6" s="48"/>
+      <c r="E6" s="48"/>
+      <c r="F6" s="48"/>
+      <c r="G6" s="48"/>
+      <c r="H6" s="50"/>
+      <c r="I6" s="48"/>
+      <c r="J6" s="48"/>
+      <c r="K6" s="48"/>
+      <c r="L6" s="48"/>
+      <c r="M6" s="48"/>
+      <c r="N6" s="48"/>
+      <c r="O6" s="43"/>
     </row>
     <row r="7" spans="1:20" ht="16.2" thickBot="1">
       <c r="A7" s="3" t="s">
@@ -2388,7 +2397,7 @@
       <c r="N7" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="O7" s="62"/>
+      <c r="O7" s="44"/>
       <c r="P7" s="32" t="s">
         <v>39</v>
       </c>
@@ -2401,35 +2410,35 @@
     </row>
     <row r="8" spans="1:20" ht="20.55" customHeight="1" thickTop="1" thickBot="1">
       <c r="A8" s="1"/>
-      <c r="B8" s="50" t="s">
+      <c r="B8" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="51"/>
-      <c r="D8" s="51"/>
-      <c r="E8" s="52"/>
-      <c r="F8" s="53" t="s">
+      <c r="C8" s="60"/>
+      <c r="D8" s="60"/>
+      <c r="E8" s="61"/>
+      <c r="F8" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="54"/>
-      <c r="H8" s="54"/>
-      <c r="I8" s="54"/>
-      <c r="J8" s="55"/>
-      <c r="K8" s="55"/>
-      <c r="L8" s="55"/>
-      <c r="M8" s="56" t="s">
+      <c r="G8" s="63"/>
+      <c r="H8" s="63"/>
+      <c r="I8" s="63"/>
+      <c r="J8" s="64"/>
+      <c r="K8" s="64"/>
+      <c r="L8" s="64"/>
+      <c r="M8" s="65" t="s">
         <v>14</v>
       </c>
-      <c r="N8" s="57"/>
+      <c r="N8" s="66"/>
       <c r="O8" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="P8" s="63" t="s">
+      <c r="P8" s="45" t="s">
         <v>38</v>
       </c>
-      <c r="Q8" s="64"/>
-      <c r="R8" s="64"/>
-      <c r="S8" s="64"/>
-      <c r="T8" s="65"/>
+      <c r="Q8" s="46"/>
+      <c r="R8" s="46"/>
+      <c r="S8" s="46"/>
+      <c r="T8" s="47"/>
     </row>
     <row r="9" spans="1:20" ht="22.05" customHeight="1" thickBot="1">
       <c r="A9" s="2" t="s">
@@ -9214,7 +9223,7 @@
         <v>298</v>
       </c>
       <c r="J195" s="33">
-        <v>-12000</v>
+        <v>575555555</v>
       </c>
       <c r="K195" s="33"/>
       <c r="L195" s="39" t="s">
@@ -9250,7 +9259,7 @@
         <v>298</v>
       </c>
       <c r="J196" s="33">
-        <v>-11720</v>
+        <v>560800000</v>
       </c>
       <c r="K196" s="33"/>
       <c r="L196" s="39" t="s">
@@ -9286,7 +9295,7 @@
         <v>298</v>
       </c>
       <c r="J197" s="33">
-        <v>-11450</v>
+        <v>619500000</v>
       </c>
       <c r="K197" s="33"/>
       <c r="L197" s="39" t="s">
@@ -9322,7 +9331,7 @@
         <v>298</v>
       </c>
       <c r="J198" s="33">
-        <v>-11190</v>
+        <v>651500000</v>
       </c>
       <c r="K198" s="33"/>
       <c r="L198" s="39" t="s">
@@ -9357,7 +9366,7 @@
       <c r="I199" s="36">
         <v>298</v>
       </c>
-      <c r="J199" s="33">
+      <c r="J199" s="68">
         <v>2583800000</v>
       </c>
       <c r="K199" s="33"/>
@@ -15875,11 +15884,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="O5:O7"/>
-    <mergeCell ref="P8:T8"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="N5:N6"/>
-    <mergeCell ref="H5:H6"/>
     <mergeCell ref="F2:N3"/>
     <mergeCell ref="D2:E3"/>
     <mergeCell ref="B8:E8"/>
@@ -15894,6 +15898,11 @@
     <mergeCell ref="K5:K6"/>
     <mergeCell ref="J5:J6"/>
     <mergeCell ref="L5:L6"/>
+    <mergeCell ref="O5:O7"/>
+    <mergeCell ref="P8:T8"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="N5:N6"/>
+    <mergeCell ref="H5:H6"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <hyperlinks>

</xml_diff>